<commit_message>
fixed minor error in test diagram.
</commit_message>
<xml_diff>
--- a/res/TestCasesMilestone.xlsx
+++ b/res/TestCasesMilestone.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="197">
   <si>
     <t>Clinic</t>
   </si>
@@ -604,6 +604,9 @@
   </si>
   <si>
     <t>Jack</t>
+  </si>
+  <si>
+    <t>assertEquals(getStaff())</t>
   </si>
 </sst>
 </file>
@@ -982,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D145"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D146" sqref="D146"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,7 +1181,7 @@
         <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>196</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -2166,6 +2169,11 @@
       </c>
       <c r="D145" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D146">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testcases milestone excel file
</commit_message>
<xml_diff>
--- a/res/TestCasesMilestone.xlsx
+++ b/res/TestCasesMilestone.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajiv\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7C5D84-5510-4474-BAFD-36E0AA8EF2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="24915" windowHeight="12600"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="255">
   <si>
     <t>Clinic</t>
   </si>
@@ -607,12 +613,186 @@
   </si>
   <si>
     <t>assertEquals(getStaff())</t>
+  </si>
+  <si>
+    <t>PatientRecord</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>testing  get most recent from patient</t>
+  </si>
+  <si>
+    <t>assertEquals(recordList.get(recordList.size() - 1), aandi.getMostRecentVisit())</t>
+  </si>
+  <si>
+    <t>assertTrue(Record("Headache, 33),aandi.getVisitRecord())</t>
+  </si>
+  <si>
+    <t>testing add record</t>
+  </si>
+  <si>
+    <t>test invalid record</t>
+  </si>
+  <si>
+    <t>aandi.addRecord("headache", -21);</t>
+  </si>
+  <si>
+    <t>IAE</t>
+  </si>
+  <si>
+    <t>testNegativeTemp</t>
+  </si>
+  <si>
+    <t>aandi.addRecord(null, 21);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testZeroTemp </t>
+  </si>
+  <si>
+    <t>assertTrue(!aandi.getVisitRecord().isEmpty)</t>
+  </si>
+  <si>
+    <t>TestMultipleVisitRecords</t>
+  </si>
+  <si>
+    <t>assertEquals(2, aandi.getVisitRecord().size());</t>
+  </si>
+  <si>
+    <t>aandi.addRecord("Feeling sick", 32.1);</t>
+  </si>
+  <si>
+    <t>Test with decimal</t>
+  </si>
+  <si>
+    <t>Patient toString with noRecord</t>
+  </si>
+  <si>
+    <t>assertEquals("aandi info", aandi.toString();</t>
+  </si>
+  <si>
+    <t>Patient toString</t>
+  </si>
+  <si>
+    <t>Multiple record toString</t>
+  </si>
+  <si>
+    <t>testRoomtoString</t>
+  </si>
+  <si>
+    <t>assertEquals("room info", room.toString();</t>
+  </si>
+  <si>
+    <t>testRoomMutlipleRectoString</t>
+  </si>
+  <si>
+    <t>testRoomNoRecToString</t>
+  </si>
+  <si>
+    <t>Doctor Prefix</t>
+  </si>
+  <si>
+    <t>testClinicalStafftoStringDoctor</t>
+  </si>
+  <si>
+    <t>assertEquals("doctor info", doctor.toString();</t>
+  </si>
+  <si>
+    <t>testClinicalStafftoStringNurse</t>
+  </si>
+  <si>
+    <t>assertEquals("nurse info", nurse.toString();</t>
+  </si>
+  <si>
+    <t>testClinicalStafftoStringNeither</t>
+  </si>
+  <si>
+    <t>assertEquals("neither info", neither.toString();</t>
+  </si>
+  <si>
+    <t>Controller test</t>
+  </si>
+  <si>
+    <t>testCommand1()</t>
+  </si>
+  <si>
+    <t>assertEquals("1\n1\nq"), out.toString();</t>
+  </si>
+  <si>
+    <t>assertEquals("2\n2\nq"), out.toString();</t>
+  </si>
+  <si>
+    <t>testCommand2()</t>
+  </si>
+  <si>
+    <t>testCommand3()</t>
+  </si>
+  <si>
+    <t>assertEquals("3\nq"), out.toString();</t>
+  </si>
+  <si>
+    <t>testCommand4()</t>
+  </si>
+  <si>
+    <t>assertEquals("4\nSteve\nJohnson\n03/05/2000\nHeadache\n32\nq"), out.toString();</t>
+  </si>
+  <si>
+    <t>testCommand5()</t>
+  </si>
+  <si>
+    <t>assertEquals("5\n\nphysician\nSteve\nJohnson\nmasters\n0123456789\nq"), out.toString();</t>
+  </si>
+  <si>
+    <t>testCommand6()</t>
+  </si>
+  <si>
+    <t>assertEquals("6\nAandi\nAcute\nHeadache\n32\nq"), out.toString();</t>
+  </si>
+  <si>
+    <t>testCommand7()</t>
+  </si>
+  <si>
+    <t>assertEquals("7\nq"), out.toString();</t>
+  </si>
+  <si>
+    <t>testCommand8()</t>
+  </si>
+  <si>
+    <t>testCommand9()</t>
+  </si>
+  <si>
+    <t>assertEquals("8\nq"), out.toString();</t>
+  </si>
+  <si>
+    <t>assertEquals("9\nq"), out.toString();</t>
+  </si>
+  <si>
+    <t>testInvalidPatient()</t>
+  </si>
+  <si>
+    <t>assertEquals("1\n12\nq"), out.toString();</t>
+  </si>
+  <si>
+    <t>assertEquals("2\n12\n3\n3\nq"), out.toString();</t>
+  </si>
+  <si>
+    <t>testInvalidRoom()</t>
+  </si>
+  <si>
+    <t>testInvalidCommand()</t>
+  </si>
+  <si>
+    <t>UnsupportedOperationException</t>
+  </si>
+  <si>
+    <t>assertEquals("12"), out.toString();</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -674,16 +854,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,14 +872,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -739,7 +920,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -811,7 +992,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -984,17 +1165,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D146"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="C181" sqref="C181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="83.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1005,13 +1186,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1484,13 +1665,13 @@
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
+      <c r="B57" t="s">
         <v>81</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" t="s">
         <v>90</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1511,13 +1692,13 @@
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1668,13 +1849,13 @@
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="3" t="s">
+      <c r="B84" t="s">
         <v>122</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C84" t="s">
         <v>121</v>
       </c>
-      <c r="D84" s="3" t="b">
+      <c r="D84" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1695,13 +1876,13 @@
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C89" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D89" s="4" t="s">
+      <c r="D89" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1766,7 +1947,7 @@
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="6" t="s">
+      <c r="B97" t="s">
         <v>134</v>
       </c>
       <c r="C97" t="s">
@@ -1777,7 +1958,7 @@
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="6" t="s">
+      <c r="B98" t="s">
         <v>135</v>
       </c>
       <c r="C98" t="s">
@@ -1788,7 +1969,7 @@
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="6" t="s">
+      <c r="B99" t="s">
         <v>136</v>
       </c>
       <c r="C99" t="s">
@@ -1799,18 +1980,18 @@
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="6" t="s">
+      <c r="B100" t="s">
         <v>137</v>
       </c>
       <c r="C100" t="s">
         <v>144</v>
       </c>
-      <c r="D100" s="7">
+      <c r="D100" s="5">
         <v>32875</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="6" t="s">
+      <c r="B101" t="s">
         <v>149</v>
       </c>
       <c r="C101" t="s">
@@ -1864,7 +2045,7 @@
       </c>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="6" t="s">
+      <c r="B110" t="s">
         <v>84</v>
       </c>
       <c r="C110" t="s">
@@ -1875,7 +2056,7 @@
       </c>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="6" t="s">
+      <c r="B111" t="s">
         <v>155</v>
       </c>
       <c r="C111" t="s">
@@ -1891,13 +2072,13 @@
       </c>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="5" t="s">
+      <c r="B114" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C114" s="4" t="s">
+      <c r="C114" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D114" s="4" t="s">
+      <c r="D114" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2046,18 +2227,18 @@
       </c>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="5" t="s">
+      <c r="B133" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C133" s="4" t="s">
+      <c r="C133" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D133" s="4" t="s">
+      <c r="D133" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="8" t="s">
+      <c r="B134" t="s">
         <v>84</v>
       </c>
       <c r="C134" t="s">
@@ -2068,7 +2249,7 @@
       </c>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="8" t="s">
+      <c r="B135" t="s">
         <v>182</v>
       </c>
       <c r="C135" t="s">
@@ -2079,7 +2260,7 @@
       </c>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B136" s="8" t="s">
+      <c r="B136" t="s">
         <v>46</v>
       </c>
       <c r="C136" t="s">
@@ -2090,7 +2271,7 @@
       </c>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="8" t="s">
+      <c r="B137" t="s">
         <v>47</v>
       </c>
       <c r="C137" t="s">
@@ -2101,7 +2282,7 @@
       </c>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="8" t="s">
+      <c r="B138" t="s">
         <v>183</v>
       </c>
       <c r="C138" t="s">
@@ -2112,7 +2293,7 @@
       </c>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B139" s="8" t="s">
+      <c r="B139" t="s">
         <v>184</v>
       </c>
       <c r="C139" t="s">
@@ -2174,6 +2355,351 @@
     <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D146">
         <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B148" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>199</v>
+      </c>
+      <c r="C149" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D149" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>202</v>
+      </c>
+      <c r="C150" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D150" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>203</v>
+      </c>
+      <c r="C151" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D151" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>206</v>
+      </c>
+      <c r="C152" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D152" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>208</v>
+      </c>
+      <c r="C153" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D153" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>210</v>
+      </c>
+      <c r="C154" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D154" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
+        <v>213</v>
+      </c>
+      <c r="C155" t="s">
+        <v>212</v>
+      </c>
+      <c r="D155" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
+        <v>214</v>
+      </c>
+      <c r="C156" t="s">
+        <v>215</v>
+      </c>
+      <c r="D156" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>216</v>
+      </c>
+      <c r="C157" t="s">
+        <v>215</v>
+      </c>
+      <c r="D157" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>217</v>
+      </c>
+      <c r="C158" t="s">
+        <v>215</v>
+      </c>
+      <c r="D158" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>218</v>
+      </c>
+      <c r="C159" t="s">
+        <v>219</v>
+      </c>
+      <c r="D159" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
+        <v>220</v>
+      </c>
+      <c r="C160" t="s">
+        <v>219</v>
+      </c>
+      <c r="D160" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>221</v>
+      </c>
+      <c r="C161" t="s">
+        <v>219</v>
+      </c>
+      <c r="D161" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B164" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>223</v>
+      </c>
+      <c r="C165" t="s">
+        <v>224</v>
+      </c>
+      <c r="D165" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B166" t="s">
+        <v>225</v>
+      </c>
+      <c r="C166" t="s">
+        <v>226</v>
+      </c>
+      <c r="D166" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
+        <v>227</v>
+      </c>
+      <c r="C167" t="s">
+        <v>228</v>
+      </c>
+      <c r="D167" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B169" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
+        <v>230</v>
+      </c>
+      <c r="C170" t="s">
+        <v>231</v>
+      </c>
+      <c r="D170" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>233</v>
+      </c>
+      <c r="C171" t="s">
+        <v>232</v>
+      </c>
+      <c r="D171" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
+        <v>234</v>
+      </c>
+      <c r="C172" t="s">
+        <v>235</v>
+      </c>
+      <c r="D172" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
+        <v>236</v>
+      </c>
+      <c r="C173" t="s">
+        <v>237</v>
+      </c>
+      <c r="D173" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
+        <v>238</v>
+      </c>
+      <c r="C174" t="s">
+        <v>239</v>
+      </c>
+      <c r="D174" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B175" t="s">
+        <v>240</v>
+      </c>
+      <c r="C175" t="s">
+        <v>241</v>
+      </c>
+      <c r="D175" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
+        <v>242</v>
+      </c>
+      <c r="C176" t="s">
+        <v>243</v>
+      </c>
+      <c r="D176" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B177" t="s">
+        <v>244</v>
+      </c>
+      <c r="C177" t="s">
+        <v>246</v>
+      </c>
+      <c r="D177" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B178" t="s">
+        <v>245</v>
+      </c>
+      <c r="C178" t="s">
+        <v>247</v>
+      </c>
+      <c r="D178" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B179" t="s">
+        <v>248</v>
+      </c>
+      <c r="C179" t="s">
+        <v>249</v>
+      </c>
+      <c r="D179" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B180" t="s">
+        <v>251</v>
+      </c>
+      <c r="C180" t="s">
+        <v>250</v>
+      </c>
+      <c r="D180" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B181" t="s">
+        <v>252</v>
+      </c>
+      <c r="C181" t="s">
+        <v>254</v>
+      </c>
+      <c r="D181" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2183,7 +2709,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2195,7 +2721,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated TestCasesMilestone Excel file
</commit_message>
<xml_diff>
--- a/res/TestCasesMilestone.xlsx
+++ b/res/TestCasesMilestone.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="317">
   <si>
     <t>Clinic</t>
   </si>
@@ -811,6 +811,162 @@
   </si>
   <si>
     <t xml:space="preserve">assertEquals("2\n12\n3\n3\nq\n", out.toString()); </t>
+  </si>
+  <si>
+    <t>MILESTONE 2</t>
+  </si>
+  <si>
+    <t>MILESTONE 1</t>
+  </si>
+  <si>
+    <t>MILESTONE 3</t>
+  </si>
+  <si>
+    <t>Clinic2</t>
+  </si>
+  <si>
+    <t>testDeactivateStaffNullArgument()</t>
+  </si>
+  <si>
+    <t>clinic.deactivateStaff(null)</t>
+  </si>
+  <si>
+    <t>testDeactivateStaff()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assertFalse(clinic.getEmployees().contains(member)); </t>
+  </si>
+  <si>
+    <t>assertEquals(5, clinic.getNumStaff());</t>
+  </si>
+  <si>
+    <t>testUnassignClinStaffNullArgument()</t>
+  </si>
+  <si>
+    <t>clinic.unassignClinStaff(amy, aandi);</t>
+  </si>
+  <si>
+    <t>testUnassignClinStaff()</t>
+  </si>
+  <si>
+    <t>assertFalse(aandi.getAllocated().contains(amy));</t>
+  </si>
+  <si>
+    <t>testListClinWithPatientInfo()</t>
+  </si>
+  <si>
+    <t>assertEquals("Clinical Staff: Amy Anguish\n"</t>
+  </si>
+  <si>
+    <t>+ " Assigned Patient: Aandi Acute", test);</t>
+  </si>
+  <si>
+    <t>testListPatientNoVisitOneYear()</t>
+  </si>
+  <si>
+    <t>assertEquals("Patient Name: Aandi Acute\n"</t>
+  </si>
+  <si>
+    <t>+ " -------------------------------", clinic.listPatientVisitMoreThanYear());</t>
+  </si>
+  <si>
+    <t>testVisitTwiceOneYear()</t>
+  </si>
+  <si>
+    <t>+ " -------------------------------", clinic.listVisitTwiceOneYear());</t>
+  </si>
+  <si>
+    <t>ControllerTest</t>
+  </si>
+  <si>
+    <t>assertEquals("10\nq\n", out.toString());</t>
+  </si>
+  <si>
+    <t>testCommand10PatientDisplay()</t>
+  </si>
+  <si>
+    <t>testCommand11DisplayMap()</t>
+  </si>
+  <si>
+    <t>testCommand12DeactivateSelectedClinStaff()</t>
+  </si>
+  <si>
+    <t>assertEquals("11\nq\n", out.toString());</t>
+  </si>
+  <si>
+    <t>assertEquals("12\n1\nq\n", out.toString());</t>
+  </si>
+  <si>
+    <t>testCommand12DeactivateSelectedNonClinStaff()</t>
+  </si>
+  <si>
+    <t>assertEquals("12\n6\nq\n", out.toString());</t>
+  </si>
+  <si>
+    <t>assertEquals("12\nq\nq\n", out.toString());</t>
+  </si>
+  <si>
+    <t>testCommand12DeactivateSelectedQuitEarly()</t>
+  </si>
+  <si>
+    <t>testCommand12DeactivateSelectedOutOfBounds()</t>
+  </si>
+  <si>
+    <t>assertEquals("12\n8\n\nq\nq\n", out.toString());</t>
+  </si>
+  <si>
+    <t>testCommand12DeactivateSelectedWrongNumberFormat()</t>
+  </si>
+  <si>
+    <t>assertEquals("12\nfour\n\nq\nq\n", out.toString());</t>
+  </si>
+  <si>
+    <t>assertEquals("13\nq\n", out.toString());</t>
+  </si>
+  <si>
+    <t>testCommand13DisplayPatientsMoreThanYear()</t>
+  </si>
+  <si>
+    <t>testCommand14DisplayPatientsTwiceOneYear()</t>
+  </si>
+  <si>
+    <t>assertEquals("14\nq\n", out.toString());</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testCommand15UnassignClinicalStaffFromPatientNoAssigned() </t>
+  </si>
+  <si>
+    <t>assertEquals("15\n1\nq\n", out.toString());</t>
+  </si>
+  <si>
+    <t>testCommand15UnassignClinicalStaffFromPatientQuitEarly()</t>
+  </si>
+  <si>
+    <t>assertEquals("15\nq\nq\n", out.toString());</t>
+  </si>
+  <si>
+    <t>testCommand15UnassignClinicalStaffFromPatientSuccessfully()</t>
+  </si>
+  <si>
+    <t>assertEquals("15\n1\n1\nq\n", out.toString());</t>
+  </si>
+  <si>
+    <t>testCommand15UnassignClinicalStaffFromPatientInvalidNumber()</t>
+  </si>
+  <si>
+    <t>assertEquals("15\n8\n\nq\nq\n", out.toString());</t>
+  </si>
+  <si>
+    <t>testCommand15UnassignClinicalStaffFromPatientInvalidNumberFormat()</t>
+  </si>
+  <si>
+    <t>assertEquals("15\nFour\n\nq\nq\n", out.toString());</t>
+  </si>
+  <si>
+    <t>testCommand16ListClinAndAssignedPatients()</t>
+  </si>
+  <si>
+    <t>assertEquals("16\nq\n", out.toString());</t>
   </si>
 </sst>
 </file>
@@ -878,7 +1034,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -886,6 +1042,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1190,26 +1354,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D186"/>
+  <dimension ref="A1:D258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="C190" sqref="C190"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D247" sqref="D247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="94.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>266</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2365,7 +2533,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>169</v>
       </c>
@@ -2376,17 +2544,20 @@
         <v>178</v>
       </c>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D146">
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>265</v>
+      </c>
       <c r="B147" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B148" s="4" t="s">
         <v>198</v>
       </c>
@@ -2397,7 +2568,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>199</v>
       </c>
@@ -2408,7 +2579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>202</v>
       </c>
@@ -2419,7 +2590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>203</v>
       </c>
@@ -2430,7 +2601,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>206</v>
       </c>
@@ -2441,7 +2612,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>208</v>
       </c>
@@ -2452,7 +2623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>210</v>
       </c>
@@ -2463,7 +2634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>213</v>
       </c>
@@ -2474,7 +2645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>214</v>
       </c>
@@ -2485,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>216</v>
       </c>
@@ -2496,7 +2667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>217</v>
       </c>
@@ -2507,7 +2678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>218</v>
       </c>
@@ -2518,7 +2689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>220</v>
       </c>
@@ -2671,7 +2842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>252</v>
       </c>
@@ -2682,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>254</v>
       </c>
@@ -2693,7 +2864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>255</v>
       </c>
@@ -2704,7 +2875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>256</v>
       </c>
@@ -2715,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>230</v>
       </c>
@@ -2726,7 +2897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>231</v>
       </c>
@@ -2737,7 +2908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>232</v>
       </c>
@@ -2748,7 +2919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>233</v>
       </c>
@@ -2759,7 +2930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>234</v>
       </c>
@@ -2770,7 +2941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>235</v>
       </c>
@@ -2780,6 +2951,531 @@
       <c r="D186" t="s">
         <v>236</v>
       </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B189" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B190" t="s">
+        <v>269</v>
+      </c>
+      <c r="C190" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="D190" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B191" t="s">
+        <v>271</v>
+      </c>
+      <c r="C191" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="D191" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B192" t="s">
+        <v>271</v>
+      </c>
+      <c r="C192" t="s">
+        <v>273</v>
+      </c>
+      <c r="D192" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D193" s="9"/>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B194" t="s">
+        <v>274</v>
+      </c>
+      <c r="C194" t="s">
+        <v>275</v>
+      </c>
+      <c r="D194" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
+        <v>276</v>
+      </c>
+      <c r="C195" t="s">
+        <v>277</v>
+      </c>
+      <c r="D195" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B196" t="s">
+        <v>278</v>
+      </c>
+      <c r="C196" t="s">
+        <v>279</v>
+      </c>
+      <c r="D196" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C197" t="s">
+        <v>280</v>
+      </c>
+      <c r="D197" s="9"/>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D198" s="9"/>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B199" t="s">
+        <v>281</v>
+      </c>
+      <c r="C199" t="s">
+        <v>282</v>
+      </c>
+      <c r="D199" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C200" t="str">
+        <f>+ "Date of Birth: 1/1/1981\n"</f>
+        <v>Date of Birth: 1/1/1981\n</v>
+      </c>
+      <c r="D200" s="9"/>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C201" t="str">
+        <f>+ "Room Number: 1\n"</f>
+        <v>Room Number: 1\n</v>
+      </c>
+      <c r="D201" s="9"/>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C202" t="str">
+        <f>+ "Assigned Staff: None\n"</f>
+        <v>Assigned Staff: None\n</v>
+      </c>
+      <c r="D202" s="9"/>
+    </row>
+    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C203" t="str">
+        <f>+ "Visit Info: \n"</f>
+        <v>Visit Info: \n</v>
+      </c>
+      <c r="D203" s="9"/>
+    </row>
+    <row r="204" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C204" t="str">
+        <f>+ " Chief Complaint: Headache\n"</f>
+        <v xml:space="preserve"> Chief Complaint: Headache\n</v>
+      </c>
+      <c r="D204" s="9"/>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C205" t="str">
+        <f>+ " Temperature: 2.0 °C\n"</f>
+        <v xml:space="preserve"> Temperature: 2.0 °C\n</v>
+      </c>
+      <c r="D205" s="9"/>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C206" t="str">
+        <f>+ " Visit Date: 11/11/2020 19:09:48\n"</f>
+        <v xml:space="preserve"> Visit Date: 11/11/2020 19:09:48\n</v>
+      </c>
+      <c r="D206" s="9"/>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C207" t="str">
+        <f>+ " ------------------------------- \n"</f>
+        <v xml:space="preserve"> ------------------------------- \n</v>
+      </c>
+      <c r="D207" s="9"/>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C208" t="str">
+        <f>+ "Patient Name: Beth Bunion\n"</f>
+        <v>Patient Name: Beth Bunion\n</v>
+      </c>
+      <c r="D208" s="9"/>
+    </row>
+    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C209" t="str">
+        <f>+ "Date of Birth: 2/2/1982\n"</f>
+        <v>Date of Birth: 2/2/1982\n</v>
+      </c>
+      <c r="D209" s="9"/>
+    </row>
+    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C210" t="str">
+        <f>+ "Room Number: 2\n"</f>
+        <v>Room Number: 2\n</v>
+      </c>
+      <c r="D210" s="9"/>
+    </row>
+    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C211" t="str">
+        <f>+ "Assigned Staff: None\n"</f>
+        <v>Assigned Staff: None\n</v>
+      </c>
+      <c r="D211" s="9"/>
+    </row>
+    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C212" t="str">
+        <f>+ "Visit Info: \n"</f>
+        <v>Visit Info: \n</v>
+      </c>
+      <c r="D212" s="9"/>
+    </row>
+    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C213" t="str">
+        <f>+ " Chief Complaint: Stomachache\n"</f>
+        <v xml:space="preserve"> Chief Complaint: Stomachache\n</v>
+      </c>
+      <c r="D213" s="9"/>
+    </row>
+    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C214" t="str">
+        <f>+ " Temperature: 10.0 °C\n"</f>
+        <v xml:space="preserve"> Temperature: 10.0 °C\n</v>
+      </c>
+      <c r="D214" s="9"/>
+    </row>
+    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C215" t="str">
+        <f>+ " Visit Date: 11/11/2019 19:09:48\n"</f>
+        <v xml:space="preserve"> Visit Date: 11/11/2019 19:09:48\n</v>
+      </c>
+      <c r="D215" s="9"/>
+    </row>
+    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C216" t="s">
+        <v>283</v>
+      </c>
+      <c r="D216" s="9"/>
+    </row>
+    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D217" s="9"/>
+    </row>
+    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
+        <v>284</v>
+      </c>
+      <c r="C218" t="s">
+        <v>282</v>
+      </c>
+      <c r="D218" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C219" t="str">
+        <f>+ "Date of Birth: 1/1/1981\n"</f>
+        <v>Date of Birth: 1/1/1981\n</v>
+      </c>
+      <c r="D219" s="9"/>
+    </row>
+    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C220" t="str">
+        <f>+ "Room Number: 1\n"</f>
+        <v>Room Number: 1\n</v>
+      </c>
+      <c r="D220" s="9"/>
+    </row>
+    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C221" t="str">
+        <f>+ "Assigned Staff: None\n"</f>
+        <v>Assigned Staff: None\n</v>
+      </c>
+      <c r="D221" s="9"/>
+    </row>
+    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C222" t="str">
+        <f>+ "Visit Info: \n"</f>
+        <v>Visit Info: \n</v>
+      </c>
+      <c r="D222" s="9"/>
+    </row>
+    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C223" t="str">
+        <f>+ " Chief Complaint: Headache\n"</f>
+        <v xml:space="preserve"> Chief Complaint: Headache\n</v>
+      </c>
+      <c r="D223" s="9"/>
+    </row>
+    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C224" t="str">
+        <f>+ " Temperature: 2.0 °C\n"</f>
+        <v xml:space="preserve"> Temperature: 2.0 °C\n</v>
+      </c>
+      <c r="D224" s="9"/>
+    </row>
+    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C225" t="str">
+        <f>+ " Visit Date: 11/11/2024 19:09:48\n\n"</f>
+        <v xml:space="preserve"> Visit Date: 11/11/2024 19:09:48\n\n</v>
+      </c>
+      <c r="D225" s="9"/>
+    </row>
+    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C226" t="str">
+        <f>+ " Chief Complaint: Headache\n"</f>
+        <v xml:space="preserve"> Chief Complaint: Headache\n</v>
+      </c>
+      <c r="D226" s="9"/>
+    </row>
+    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C227" t="str">
+        <f>+ " Temperature: 2.0 °C\n"</f>
+        <v xml:space="preserve"> Temperature: 2.0 °C\n</v>
+      </c>
+      <c r="D227" s="9"/>
+    </row>
+    <row r="228" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C228" t="str">
+        <f>+ " Visit Date: 11/12/2024 19:09:48\n"</f>
+        <v xml:space="preserve"> Visit Date: 11/12/2024 19:09:48\n</v>
+      </c>
+      <c r="D228" s="9"/>
+    </row>
+    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C229" t="s">
+        <v>285</v>
+      </c>
+      <c r="D229" s="9"/>
+    </row>
+    <row r="230" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D230" s="9"/>
+    </row>
+    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B231" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="232" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B232" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="C232" t="s">
+        <v>287</v>
+      </c>
+      <c r="D232" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B233" t="s">
+        <v>289</v>
+      </c>
+      <c r="C233" t="s">
+        <v>291</v>
+      </c>
+      <c r="D233" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B234" t="s">
+        <v>290</v>
+      </c>
+      <c r="C234" t="s">
+        <v>292</v>
+      </c>
+      <c r="D234" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B235" t="s">
+        <v>293</v>
+      </c>
+      <c r="C235" t="s">
+        <v>294</v>
+      </c>
+      <c r="D235" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B236" t="s">
+        <v>296</v>
+      </c>
+      <c r="C236" t="s">
+        <v>295</v>
+      </c>
+      <c r="D236" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B237" t="s">
+        <v>297</v>
+      </c>
+      <c r="C237" t="s">
+        <v>298</v>
+      </c>
+      <c r="D237" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B238" t="s">
+        <v>299</v>
+      </c>
+      <c r="C238" t="s">
+        <v>300</v>
+      </c>
+      <c r="D238" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B239" t="s">
+        <v>302</v>
+      </c>
+      <c r="C239" t="s">
+        <v>301</v>
+      </c>
+      <c r="D239" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B240" t="s">
+        <v>303</v>
+      </c>
+      <c r="C240" t="s">
+        <v>304</v>
+      </c>
+      <c r="D240" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B241" t="s">
+        <v>305</v>
+      </c>
+      <c r="C241" t="s">
+        <v>306</v>
+      </c>
+      <c r="D241" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B242" t="s">
+        <v>307</v>
+      </c>
+      <c r="C242" t="s">
+        <v>308</v>
+      </c>
+      <c r="D242" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B243" t="s">
+        <v>309</v>
+      </c>
+      <c r="C243" t="s">
+        <v>310</v>
+      </c>
+      <c r="D243" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B244" t="s">
+        <v>311</v>
+      </c>
+      <c r="C244" t="s">
+        <v>312</v>
+      </c>
+      <c r="D244" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B245" t="s">
+        <v>313</v>
+      </c>
+      <c r="C245" t="s">
+        <v>314</v>
+      </c>
+      <c r="D245" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B246" t="s">
+        <v>315</v>
+      </c>
+      <c r="C246" t="s">
+        <v>316</v>
+      </c>
+      <c r="D246" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D247" s="9"/>
+    </row>
+    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D248" s="9"/>
+    </row>
+    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D249" s="9"/>
+    </row>
+    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D250" s="9"/>
+    </row>
+    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D251" s="8"/>
+    </row>
+    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D252" s="8"/>
+    </row>
+    <row r="253" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D253" s="8"/>
+    </row>
+    <row r="254" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D254" s="8"/>
+    </row>
+    <row r="255" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D255" s="8"/>
+    </row>
+    <row r="256" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D256" s="8"/>
+    </row>
+    <row r="257" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D257" s="8"/>
+    </row>
+    <row r="258" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D258" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>